<commit_message>
Update buttons in detail page and bookmark list in mypage
</commit_message>
<xml_diff>
--- a/documents/nodejs 통신값.xlsx
+++ b/documents/nodejs 통신값.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\OneDrive\Readers\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CAU\Documents\GitHub\Readers\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3012" windowWidth="21600" windowHeight="11388"/>
+    <workbookView xWindow="0" yWindow="3015" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -773,21 +773,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.3984375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="41.09765625" customWidth="1"/>
-    <col min="4" max="4" width="77.8984375" customWidth="1"/>
-    <col min="5" max="5" width="40.09765625" style="22" customWidth="1"/>
-    <col min="6" max="11" width="7.59765625" customWidth="1"/>
+    <col min="2" max="2" width="18.375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="41.125" customWidth="1"/>
+    <col min="4" max="4" width="77.875" customWidth="1"/>
+    <col min="5" max="5" width="40.125" style="22" customWidth="1"/>
+    <col min="6" max="11" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" customHeight="1"/>
     <row r="2" spans="1:5" ht="16.5" customHeight="1" thickBot="1"/>
-    <row r="3" spans="1:5" s="5" customFormat="1" ht="18" thickBot="1">
+    <row r="3" spans="1:5" s="5" customFormat="1" ht="17.25" thickBot="1">
       <c r="A3" s="7"/>
       <c r="B3" s="8"/>
       <c r="C3" s="9" t="s">
@@ -800,7 +802,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" ht="17.399999999999999">
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="16.5">
       <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
@@ -813,7 +815,7 @@
       <c r="D4" s="12"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" ht="17.399999999999999">
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="16.5">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
         <v>3</v>
@@ -824,7 +826,7 @@
       <c r="D5" s="12"/>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" ht="17.399999999999999">
+    <row r="6" spans="1:5" s="4" customFormat="1" ht="16.5">
       <c r="A6" s="13"/>
       <c r="B6" s="14" t="s">
         <v>4</v>
@@ -837,7 +839,7 @@
       </c>
       <c r="E6" s="25"/>
     </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" ht="17.399999999999999">
+    <row r="7" spans="1:5" s="2" customFormat="1" ht="16.5">
       <c r="A7" s="16" t="s">
         <v>7</v>
       </c>
@@ -850,7 +852,7 @@
       <c r="D7" s="18"/>
       <c r="E7" s="26"/>
     </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" ht="17.399999999999999">
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="16.5">
       <c r="A8" s="10"/>
       <c r="B8" s="11" t="s">
         <v>3</v>
@@ -861,7 +863,7 @@
       <c r="D8" s="12"/>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" ht="17.399999999999999">
+    <row r="9" spans="1:5" s="4" customFormat="1" ht="16.5">
       <c r="A9" s="13"/>
       <c r="B9" s="14" t="s">
         <v>4</v>
@@ -874,7 +876,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" ht="17.399999999999999">
+    <row r="10" spans="1:5" s="2" customFormat="1" ht="16.5">
       <c r="A10" s="16" t="s">
         <v>11</v>
       </c>
@@ -887,7 +889,7 @@
       <c r="D10" s="18"/>
       <c r="E10" s="26"/>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" ht="17.399999999999999">
+    <row r="11" spans="1:5" s="3" customFormat="1" ht="16.5">
       <c r="A11" s="10"/>
       <c r="B11" s="11" t="s">
         <v>3</v>
@@ -898,7 +900,7 @@
       <c r="D11" s="12"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" s="4" customFormat="1" ht="17.399999999999999">
+    <row r="12" spans="1:5" s="4" customFormat="1" ht="16.5">
       <c r="A12" s="13"/>
       <c r="B12" s="14" t="s">
         <v>4</v>
@@ -909,7 +911,7 @@
       <c r="D12" s="15"/>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" ht="17.399999999999999">
+    <row r="13" spans="1:5" s="2" customFormat="1" ht="16.5">
       <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
@@ -922,7 +924,7 @@
       <c r="D13" s="18"/>
       <c r="E13" s="26"/>
     </row>
-    <row r="14" spans="1:5" s="3" customFormat="1" ht="17.399999999999999">
+    <row r="14" spans="1:5" s="3" customFormat="1" ht="16.5">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>3</v>
@@ -933,7 +935,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" ht="17.399999999999999">
+    <row r="15" spans="1:5" s="4" customFormat="1" ht="16.5">
       <c r="A15" s="13"/>
       <c r="B15" s="14" t="s">
         <v>4</v>
@@ -946,7 +948,7 @@
       </c>
       <c r="E15" s="25"/>
     </row>
-    <row r="16" spans="1:5" s="2" customFormat="1" ht="17.399999999999999">
+    <row r="16" spans="1:5" s="2" customFormat="1" ht="16.5">
       <c r="A16" s="16" t="s">
         <v>18</v>
       </c>
@@ -961,7 +963,7 @@
       </c>
       <c r="E16" s="26"/>
     </row>
-    <row r="17" spans="1:5" s="3" customFormat="1" ht="34.799999999999997">
+    <row r="17" spans="1:5" s="3" customFormat="1" ht="33">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
         <v>22</v>
@@ -974,7 +976,7 @@
       </c>
       <c r="E17" s="24"/>
     </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" ht="34.799999999999997">
+    <row r="18" spans="1:5" s="3" customFormat="1" ht="33">
       <c r="A18" s="10"/>
       <c r="B18" s="11" t="s">
         <v>24</v>
@@ -987,7 +989,7 @@
       </c>
       <c r="E18" s="24"/>
     </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" ht="17.399999999999999">
+    <row r="19" spans="1:5" s="3" customFormat="1" ht="16.5">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
         <v>36</v>
@@ -1000,7 +1002,7 @@
       </c>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:5" s="3" customFormat="1" ht="17.399999999999999">
+    <row r="20" spans="1:5" s="3" customFormat="1" ht="16.5">
       <c r="A20" s="10"/>
       <c r="B20" s="11" t="s">
         <v>37</v>
@@ -1013,7 +1015,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" s="4" customFormat="1" ht="17.399999999999999">
+    <row r="21" spans="1:5" s="4" customFormat="1" ht="16.5">
       <c r="A21" s="13"/>
       <c r="B21" s="14" t="s">
         <v>40</v>
@@ -1026,7 +1028,7 @@
       </c>
       <c r="E21" s="25"/>
     </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" ht="17.399999999999999">
+    <row r="22" spans="1:5" s="2" customFormat="1" ht="16.5">
       <c r="A22" s="16" t="s">
         <v>35</v>
       </c>
@@ -1043,7 +1045,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="4" customFormat="1" ht="34.799999999999997">
+    <row r="23" spans="1:5" s="4" customFormat="1" ht="33">
       <c r="A23" s="13"/>
       <c r="B23" s="14" t="s">
         <v>38</v>

</xml_diff>